<commit_message>
fix(Klein): use EMK for c*phi_E in Leerlaufversuch
</commit_message>
<xml_diff>
--- a/Klein/excel/Leerlaufversuch.xlsx
+++ b/Klein/excel/Leerlaufversuch.xlsx
@@ -474,7 +474,7 @@
         <v>0.42</v>
       </c>
       <c r="E2" t="n">
-        <v>0.002388</v>
+        <v>0.1332</v>
       </c>
     </row>
     <row r="3">
@@ -491,7 +491,7 @@
         <v>0.39</v>
       </c>
       <c r="E3" t="n">
-        <v>0.0024025</v>
+        <v>0.132</v>
       </c>
     </row>
     <row r="4">
@@ -508,7 +508,7 @@
         <v>0.357</v>
       </c>
       <c r="E4" t="n">
-        <v>0.002433333333333333</v>
+        <v>0.132</v>
       </c>
     </row>
     <row r="5">
@@ -525,7 +525,7 @@
         <v>0.327</v>
       </c>
       <c r="E5" t="n">
-        <v>0.0025</v>
+        <v>0.1329</v>
       </c>
     </row>
     <row r="6">
@@ -542,7 +542,7 @@
         <v>0.276</v>
       </c>
       <c r="E6" t="n">
-        <v>0.00268</v>
+        <v>0.132</v>
       </c>
     </row>
   </sheetData>

</xml_diff>